<commit_message>
Push all the changes to git
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANDRASEKHARJANGA\PycharmProjects\TestProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB3CCFB-7710-4789-966D-486571062E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5475043-CD6A-4953-BD5E-032F3E6EB029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{1C11EC09-AC7C-4D50-BA59-48AF67F2E22B}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>